<commit_message>
Updated Task list sheet
</commit_message>
<xml_diff>
--- a/docs/User Story Titles, Estimates, and Priorities.xlsx
+++ b/docs/User Story Titles, Estimates, and Priorities.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27430"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14420" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>US Post product info</t>
   </si>
@@ -91,6 +91,12 @@
   </si>
   <si>
     <t>User Story</t>
+  </si>
+  <si>
+    <t>Home page?</t>
+  </si>
+  <si>
+    <t>Assignment Group</t>
   </si>
 </sst>
 </file>
@@ -127,20 +133,41 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -161,9 +188,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="15">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -509,19 +542,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C1048576"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="59.83203125" customWidth="1"/>
     <col min="2" max="2" width="17.1640625" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -531,167 +565,210 @@
       <c r="C1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="17">
-      <c r="A2" s="1" t="s">
+      <c r="D1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" s="3" customFormat="1" ht="17">
+      <c r="A2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C2" s="3">
+        <v>10</v>
+      </c>
+      <c r="D2" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="3" customFormat="1" ht="17">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="3">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3">
+        <v>10</v>
+      </c>
+      <c r="D3" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="3" customFormat="1" ht="17">
+      <c r="A4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="3">
+        <v>2</v>
+      </c>
+      <c r="C4" s="3">
+        <v>10</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="3" customFormat="1" ht="17">
+      <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2">
+      <c r="B5" s="3">
         <v>0.5</v>
       </c>
-      <c r="C2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="17">
-      <c r="A3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3">
+      <c r="C5" s="3">
+        <v>10</v>
+      </c>
+      <c r="D5" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="3" customFormat="1" ht="17">
+      <c r="A6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="3">
+        <v>1</v>
+      </c>
+      <c r="C6" s="3">
+        <v>10</v>
+      </c>
+      <c r="D6" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="3" customFormat="1" ht="17">
+      <c r="A7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="3">
+        <v>1</v>
+      </c>
+      <c r="C7" s="3">
+        <v>10</v>
+      </c>
+      <c r="D7" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="3" customFormat="1" ht="17">
+      <c r="A8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="3">
         <v>0.5</v>
       </c>
-      <c r="C3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="17">
-      <c r="A4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="17">
-      <c r="A5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="17">
-      <c r="A6" s="1" t="s">
+      <c r="C8" s="3">
+        <v>20</v>
+      </c>
+      <c r="D8" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="3" customFormat="1" ht="17">
+      <c r="A9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="3">
+        <v>1</v>
+      </c>
+      <c r="C9" s="3">
+        <v>10</v>
+      </c>
+      <c r="D9" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="3" customFormat="1" ht="17">
+      <c r="A10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="3">
+        <v>1</v>
+      </c>
+      <c r="C10" s="3">
+        <v>10</v>
+      </c>
+      <c r="D10" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" s="3" customFormat="1" ht="17">
+      <c r="A11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C11" s="3">
+        <v>20</v>
+      </c>
+      <c r="D11" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" s="3" customFormat="1" ht="17">
+      <c r="A12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C12" s="3">
+        <v>20</v>
+      </c>
+      <c r="D12" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" s="3" customFormat="1" ht="17">
+      <c r="A13" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="3">
+        <v>2</v>
+      </c>
+      <c r="C13" s="3">
+        <v>10</v>
+      </c>
+      <c r="D13" s="3">
         <v>4</v>
       </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="17">
-      <c r="A7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="C7">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="17">
-      <c r="A8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="C8">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="17">
-      <c r="A9" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9">
-        <v>2</v>
-      </c>
-      <c r="C9">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="17">
-      <c r="A10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10">
-        <v>2</v>
-      </c>
-      <c r="C10">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="17">
-      <c r="A11" s="1" t="s">
+    </row>
+    <row r="14" spans="1:4" s="3" customFormat="1" ht="17">
+      <c r="A14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="3">
+        <v>1</v>
+      </c>
+      <c r="C14" s="3">
+        <v>30</v>
+      </c>
+      <c r="D14" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="17">
+      <c r="A15" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B11">
+      <c r="B15" s="7">
         <v>3</v>
       </c>
-      <c r="C11">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="17">
-      <c r="A12" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B12">
-        <v>0.5</v>
-      </c>
-      <c r="C12">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="17">
-      <c r="A13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13">
-        <v>0.5</v>
-      </c>
-      <c r="C13">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="17">
-      <c r="A14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14">
-        <v>0.5</v>
-      </c>
-      <c r="C14">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="17">
-      <c r="A15" s="1" t="s">
+      <c r="C15" s="7">
+        <v>10</v>
+      </c>
+      <c r="D15" s="7"/>
+    </row>
+    <row r="16" spans="1:4" ht="17">
+      <c r="A16" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B15">
+      <c r="B16">
         <v>1.5</v>
-      </c>
-      <c r="C15">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="17">
-      <c r="A16" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B16">
-        <v>2</v>
       </c>
       <c r="C16">
         <v>20</v>
@@ -699,10 +776,10 @@
     </row>
     <row r="17" spans="1:3" ht="17">
       <c r="A17" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B17">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C17">
         <v>20</v>
@@ -710,10 +787,10 @@
     </row>
     <row r="18" spans="1:3" ht="17">
       <c r="A18" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B18">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C18">
         <v>20</v>
@@ -721,7 +798,7 @@
     </row>
     <row r="19" spans="1:3" ht="17">
       <c r="A19" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19">
         <v>5</v>
@@ -732,23 +809,23 @@
     </row>
     <row r="20" spans="1:3" ht="17">
       <c r="A20" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20">
+        <v>5</v>
+      </c>
+      <c r="C20">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" s="5" customFormat="1" ht="17">
+      <c r="A21" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B20">
-        <v>1</v>
-      </c>
-      <c r="C20">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="17">
-      <c r="A21" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B21">
-        <v>1</v>
-      </c>
-      <c r="C21">
+      <c r="B21" s="5">
+        <v>1</v>
+      </c>
+      <c r="C21" s="5">
         <v>30</v>
       </c>
     </row>
@@ -763,10 +840,14 @@
         <v>30</v>
       </c>
     </row>
+    <row r="24" spans="1:3" ht="17">
+      <c r="A24" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState ref="A2:C98">
-    <sortCondition ref="C2:C98"/>
-    <sortCondition ref="B2:B98"/>
+  <sortState ref="A2:D22">
+    <sortCondition ref="D2:D22"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>